<commit_message>
updating parameter mapping source and package file with new method column
</commit_message>
<xml_diff>
--- a/inst/extdata/ParameterMapping_final.xlsx
+++ b/inst/extdata/ParameterMapping_final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\1 ACASAK\MassWateR\Design\Example input files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C319763-CAA1-423C-A5C4-F97E3DB97671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B92B094D-7D92-4A93-8E7C-9DCA19D097DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1176" yWindow="1224" windowWidth="19452" windowHeight="9312" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{178F5C9C-564C-4FDF-AA7C-E06704DA2294}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
       </xcalcf:calcFeatures>
@@ -57,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="85">
   <si>
     <t>Water Temp</t>
   </si>
@@ -248,6 +250,9 @@
     <t>uS/cm, mS/cm, S/m</t>
   </si>
   <si>
+    <t>ppth, PSU, PSS, g/kg</t>
+  </si>
+  <si>
     <t>Chl a</t>
   </si>
   <si>
@@ -272,6 +277,9 @@
     <t>Chlorophyll a (probe)</t>
   </si>
   <si>
+    <t>blank</t>
+  </si>
+  <si>
     <t>If s.u. is used, switch it to blank for WQX.</t>
   </si>
   <si>
@@ -299,22 +307,13 @@
     <t>PON</t>
   </si>
   <si>
-    <t>Air Temp</t>
-  </si>
-  <si>
-    <t>Temperature, air</t>
-  </si>
-  <si>
-    <t>Gage</t>
-  </si>
-  <si>
-    <t>Height, gage</t>
-  </si>
-  <si>
-    <t>ppt, ppth, PSU, PSS, g/kg</t>
-  </si>
-  <si>
-    <t>NA, s.u.</t>
+    <t>Method</t>
+  </si>
+  <si>
+    <t>Lab</t>
+  </si>
+  <si>
+    <t>InSitu</t>
   </si>
 </sst>
 </file>
@@ -707,24 +706,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84032A94-31D2-4739-AFB0-3D4EF11D54E8}">
-  <dimension ref="A1:E42"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomRight" activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" customWidth="1"/>
-    <col min="2" max="2" width="28.109375" customWidth="1"/>
-    <col min="3" max="3" width="58.33203125" customWidth="1"/>
-    <col min="4" max="4" width="59.33203125" customWidth="1"/>
+    <col min="1" max="1" width="18.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="3" max="3" width="58.28515625" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="5" width="59.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -734,11 +734,14 @@
       <c r="C1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -748,573 +751,662 @@
       <c r="C2" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>80</v>
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>84</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="C5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+      <c r="D5" t="s">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>3</v>
+      </c>
+      <c r="D6" t="s">
+        <v>84</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="C7" t="s">
-        <v>3</v>
-      </c>
-      <c r="D7" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>22</v>
+        <v>5</v>
       </c>
       <c r="C9" t="s">
-        <v>22</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="D9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>5</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>52</v>
+      <c r="B11" s="4" t="s">
+        <v>50</v>
       </c>
       <c r="C11" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+        <v>49</v>
+      </c>
+      <c r="D11" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="C12" t="s">
-        <v>49</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+      <c r="D12" t="s">
+        <v>83</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>66</v>
+        <v>11</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>51</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>83</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="2" t="s">
-        <v>32</v>
+      <c r="B14" s="4" t="s">
+        <v>38</v>
       </c>
       <c r="C14" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>38</v>
+      <c r="B15" s="2" t="s">
+        <v>39</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>83</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>41</v>
+      </c>
+      <c r="D16" t="s">
+        <v>83</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>11</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>41</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>34</v>
+      </c>
+      <c r="D17" t="s">
+        <v>83</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>25</v>
+      <c r="B18" s="4" t="s">
+        <v>81</v>
       </c>
       <c r="C18" t="s">
-        <v>34</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>80</v>
+      </c>
+      <c r="D18" t="s">
+        <v>83</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>11</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>31</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>31</v>
       </c>
       <c r="C19" t="s">
-        <v>78</v>
-      </c>
-      <c r="D19" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+      <c r="D19" t="s">
+        <v>83</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>31</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>42</v>
+      </c>
+      <c r="D20" t="s">
+        <v>83</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>79</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="D21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>77</v>
+        <v>6</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>6</v>
       </c>
       <c r="C22" t="s">
-        <v>77</v>
-      </c>
-      <c r="D22" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>6</v>
+      </c>
+      <c r="D22" t="s">
+        <v>83</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>6</v>
-      </c>
-      <c r="B23" s="2" t="s">
-        <v>6</v>
+        <v>78</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>78</v>
       </c>
       <c r="C23" t="s">
-        <v>6</v>
-      </c>
-      <c r="D23" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+      <c r="D23" t="s">
+        <v>83</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>76</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>76</v>
+        <v>46</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>4</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
-      </c>
-      <c r="D24" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>36</v>
+      </c>
+      <c r="D24" t="s">
+        <v>83</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>46</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>4</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>36</v>
-      </c>
-      <c r="D25" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D25" t="s">
+        <v>83</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>46</v>
+        <v>18</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C26" t="s">
-        <v>40</v>
-      </c>
-      <c r="D26" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>18</v>
+      </c>
+      <c r="D26" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>18</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>18</v>
+      <c r="B27" s="4" t="s">
+        <v>19</v>
       </c>
       <c r="C27" t="s">
-        <v>18</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>43</v>
+      </c>
+      <c r="D27" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>18</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>19</v>
+        <v>12</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="C28" t="s">
-        <v>43</v>
-      </c>
-      <c r="D28" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="D28" t="s">
+        <v>83</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>12</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>63</v>
+        <v>70</v>
       </c>
       <c r="C29" t="s">
-        <v>27</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+      <c r="D29" t="s">
+        <v>84</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>12</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C31" t="s">
+        <v>30</v>
+      </c>
+      <c r="D31" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C30" t="s">
-        <v>70</v>
-      </c>
-      <c r="D30" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>12</v>
-      </c>
-      <c r="B31" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>21</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C32" t="s">
-        <v>30</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+        <v>16</v>
+      </c>
+      <c r="D32" t="s">
+        <v>83</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>21</v>
       </c>
-      <c r="B33" s="2" t="s">
-        <v>16</v>
+      <c r="B33" s="4" t="s">
+        <v>17</v>
       </c>
       <c r="C33" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+        <v>17</v>
+      </c>
+      <c r="D33" t="s">
+        <v>83</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>21</v>
+        <v>76</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="C34" t="s">
-        <v>17</v>
-      </c>
-      <c r="D34" s="1" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>76</v>
+      </c>
+      <c r="D34" t="s">
+        <v>83</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>74</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>74</v>
+        <v>20</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C35" t="s">
-        <v>74</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>44</v>
+      </c>
+      <c r="D35" t="s">
+        <v>84</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>20</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C36" t="s">
-        <v>44</v>
-      </c>
-      <c r="D36" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>45</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>20</v>
       </c>
-      <c r="B37" s="2" t="s">
-        <v>65</v>
+      <c r="B37" s="4" t="s">
+        <v>75</v>
       </c>
       <c r="C37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D37" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>83</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>20</v>
+        <v>77</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
       <c r="C38" t="s">
-        <v>73</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="D38" t="s">
+        <v>83</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>75</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>75</v>
+        <v>23</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="C39" t="s">
-        <v>75</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+        <v>23</v>
+      </c>
+      <c r="D39" t="s">
+        <v>84</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>23</v>
-      </c>
-      <c r="B40" s="2" t="s">
-        <v>23</v>
+        <v>47</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>47</v>
       </c>
       <c r="C40" t="s">
-        <v>23</v>
-      </c>
-      <c r="D40" s="1" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
         <v>47</v>
       </c>
-      <c r="B41" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" t="s">
-        <v>47</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>82</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="C42" t="s">
-        <v>83</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="D40" t="s">
+        <v>84</v>
+      </c>
+      <c r="E40" s="1" t="s">
         <v>59</v>
       </c>
     </row>

</xml_diff>